<commit_message>
done: all docs, fix SRS issues
</commit_message>
<xml_diff>
--- a/pm-doc/week2/项目周报_G06_Week2.xlsx
+++ b/pm-doc/week2/项目周报_G06_Week2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HaHaHaHa/Desktop/AchieveIt-Docs/pm-doc/week2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B10327D-55E7-BB41-9929-F81B68501068}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A35829E-330D-BB41-BB13-041BBC75D889}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{E1701B8E-C766-4E73-A45B-EFE082D1FEF4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>项目所处阶段</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,16 +43,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>提示：项目进展报告应该包括以下的信息：
-1/ 前几周内发现的新问题的描述，包括新发现的bug和还没有解决的设计问题。 
-2/ 在过去几周内已经解决的问题的描述，包括已经修复的bug以及如何修复的说明，还包括一些已经解决的设计问题及如何解决的。 
-3/一直没有的到解决的问题。 
-4/下周的计划，规划每个成员的具体工作和目标。 
-5/上周计划实现的评估。 
-6/项目当前状态 是否正常</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>问题（风险）应对策略</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -65,7 +55,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>目前项目进度稳定可控，已完成需求分析及需求文档的撰写</t>
+    <t>前后端联通不畅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>采用easyAPI进行API的命名、参数、返回值的统一定义，由PM和架构进行统一审核</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>见《第二周工作总结》（点击右边图标，右键-文档对象-打开）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -73,7 +71,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,15 +96,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -122,7 +111,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -145,50 +134,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -201,19 +153,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -231,6 +174,79 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>4025900</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>139700</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>4991100</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>749300</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Object 1" descr="第二周工作总结word" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62E606CA-3876-164B-B551-89C3E9AC395F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects>
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="808080"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -529,11 +545,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786FF6F8-AF56-4101-8D3D-B99B601011C6}">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786FF6F8-AF56-4101-8D3D-B99B601011C6}">
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -550,53 +566,78 @@
     <col min="11" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="116" customHeight="1">
-      <c r="A1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="4"/>
+    <row r="1" spans="1:2" ht="26" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="26" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>1</v>
+    <row r="2" spans="1:2" ht="42.5" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="42.5" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
+    <row r="3" spans="1:2" ht="72" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="47" customHeight="1">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="268" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="1:2" ht="54.5" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="47" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="54.5" customHeight="1">
-      <c r="A6" s="6" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <oleObjects>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="文档" dvAspect="DVASPECT_ICON" shapeId="1025" r:id="rId4">
+          <objectPr defaultSize="0" altText="第二周工作总结word" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>4025900</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>139700</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>4991100</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>749300</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="文档" dvAspect="DVASPECT_ICON" shapeId="1025" r:id="rId4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </oleObjects>
 </worksheet>
 </file>
</xml_diff>